<commit_message>
optimization: Encapsulate common database functions to a base class & fix last commit error
</commit_message>
<xml_diff>
--- a/resource/excel/common/IObject.xlsx
+++ b/resource/excel/common/IObject.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="7260"/>
+    <workbookView windowWidth="26136" windowHeight="16260"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Id</t>
   </si>
   <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>ConfigID</t>
+  </si>
+  <si>
+    <t>ClassName</t>
+  </si>
+  <si>
+    <t>SceneID</t>
+  </si>
+  <si>
+    <t>GroupID</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>MoveTo</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>MasterID</t>
+  </si>
+  <si>
+    <t>Disable</t>
+  </si>
+  <si>
+    <t>Connection</t>
+  </si>
+  <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>vector3</t>
+  </si>
+  <si>
+    <t>object</t>
   </si>
   <si>
     <t>Public</t>
@@ -49,7 +97,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -60,7 +108,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -79,10 +127,38 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -90,14 +166,22 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -105,7 +189,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -113,7 +197,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -121,7 +205,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -129,96 +213,60 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -244,13 +292,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -268,24 +358,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -304,18 +406,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -328,36 +418,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -376,24 +442,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -412,12 +466,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -429,7 +477,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -453,13 +501,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -469,6 +517,36 @@
     </border>
     <border>
       <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
@@ -490,8 +568,51 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -525,21 +646,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -598,218 +704,245 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1078,67 +1211,417 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89090909090909" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="5" width="11.4444444444444" customWidth="1"/>
+    <col min="6" max="6" width="15.3333333333333" customWidth="1"/>
+    <col min="7" max="7" width="14.1111111111111" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="17.7777777777778" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="11" max="11" width="20.8888888888889" customWidth="1"/>
+    <col min="12" max="12" width="26.1111111111111" customWidth="1"/>
+    <col min="13" max="13" width="23.8888888888889" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
+    <row r="2" spans="1:13">
+      <c r="A2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
+    <row r="3" spans="1:13">
+      <c r="A3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7">
+        <v>1</v>
+      </c>
+      <c r="H3" s="9">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7">
+        <v>1</v>
+      </c>
+      <c r="L3" s="7">
+        <v>0</v>
+      </c>
+      <c r="M3" s="7">
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
+    <row r="4" spans="1:13">
+      <c r="A4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1</v>
+      </c>
+      <c r="G4" s="7">
+        <v>1</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7">
+        <v>1</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0</v>
+      </c>
+      <c r="K4" s="7">
+        <v>1</v>
+      </c>
+      <c r="L4" s="7">
+        <v>1</v>
+      </c>
+      <c r="M4" s="7">
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
+    <row r="5" spans="1:13">
+      <c r="A5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0</v>
+      </c>
+      <c r="G5" s="9">
+        <v>0</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7">
+        <v>0</v>
+      </c>
+      <c r="L5" s="7">
+        <v>0</v>
+      </c>
+      <c r="M5" s="7">
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
+    <row r="6" spans="1:13">
+      <c r="A6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0</v>
+      </c>
+      <c r="H6" s="9">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7">
+        <v>1</v>
+      </c>
+      <c r="J6" s="9">
+        <v>0</v>
+      </c>
+      <c r="K6" s="9">
+        <v>0</v>
+      </c>
+      <c r="L6" s="9">
+        <v>0</v>
+      </c>
+      <c r="M6" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
+    <row r="7" spans="1:13">
+      <c r="A7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
+        <v>0</v>
+      </c>
+      <c r="H7" s="9">
+        <v>0</v>
+      </c>
+      <c r="I7" s="9">
+        <v>0</v>
+      </c>
+      <c r="J7" s="9">
+        <v>0</v>
+      </c>
+      <c r="K7" s="9">
+        <v>0</v>
+      </c>
+      <c r="L7" s="9">
+        <v>0</v>
+      </c>
+      <c r="M7" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
+    <row r="8" spans="1:13">
+      <c r="A8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+      <c r="H8" s="9">
+        <v>0</v>
+      </c>
+      <c r="I8" s="9">
+        <v>0</v>
+      </c>
+      <c r="J8" s="9">
+        <v>0</v>
+      </c>
+      <c r="K8" s="9">
+        <v>0</v>
+      </c>
+      <c r="L8" s="9">
+        <v>0</v>
+      </c>
+      <c r="M8" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="3" t="s">
-        <v>8</v>
+    <row r="9" spans="1:13">
+      <c r="A9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="9">
+        <v>0</v>
+      </c>
+      <c r="I9" s="9">
+        <v>0</v>
+      </c>
+      <c r="J9" s="9">
+        <v>0</v>
+      </c>
+      <c r="K9" s="9">
+        <v>0</v>
+      </c>
+      <c r="L9" s="9">
+        <v>0</v>
+      </c>
+      <c r="M9" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="10" ht="15.25" spans="1:1">
-      <c r="A10" s="4" t="s">
-        <v>9</v>
-      </c>
+    <row r="10" ht="15.15" spans="1:13">
+      <c r="A10" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9"/>
+  <dataValidations count="2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:J1 K1:L1 M1 A7:A9"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2 B3 I3 J3 K3 L3 M3 I4 J4 K4 L4 M4 I10:J10 K10:L10 M10 B7:B9 C7:C9 D7:D9 M5:M6 M7:M9 E7:F9 G7:H9 I7:J9 K7:L9 G3:H6 I5:J6 K5:L6">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>